<commit_message>
ID:OMS-CIL-02-->Update CIL with data& RTM
</commit_message>
<xml_diff>
--- a/PM/OnlineMobileStore_CIL.xlsx
+++ b/PM/OnlineMobileStore_CIL.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F31197-4987-4F88-858D-626F5398928A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007431E6-91D2-49C4-A4CB-93B3C427A39E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -66,34 +66,116 @@
     <t>SIQ</t>
   </si>
   <si>
-    <t>Change Request</t>
-  </si>
-  <si>
-    <t>Review Process</t>
-  </si>
-  <si>
-    <t>Problem Management</t>
-  </si>
-  <si>
-    <t>CI_00</t>
-  </si>
-  <si>
-    <t>CI_01</t>
-  </si>
-  <si>
-    <t>CI_02</t>
-  </si>
-  <si>
-    <t>CI_03</t>
-  </si>
-  <si>
-    <t>CI_04</t>
-  </si>
-  <si>
-    <t>CI_05</t>
-  </si>
-  <si>
     <t>Owner</t>
+  </si>
+  <si>
+    <t>Mario Adel</t>
+  </si>
+  <si>
+    <t>Ghada Hassan</t>
+  </si>
+  <si>
+    <t>Sama Wagdy
+Salma Khaled
+Ghada Hassan
+Salma Mohammed</t>
+  </si>
+  <si>
+    <t>v1.0</t>
+  </si>
+  <si>
+    <t>/Online_Mobile_Store/PM/PMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changes Template </t>
+  </si>
+  <si>
+    <t>Issues template</t>
+  </si>
+  <si>
+    <t>Salma Khaled</t>
+  </si>
+  <si>
+    <t>Review template</t>
+  </si>
+  <si>
+    <t>OMS_CI_01</t>
+  </si>
+  <si>
+    <t>OMS_CI_02</t>
+  </si>
+  <si>
+    <t>OMS_CI_03</t>
+  </si>
+  <si>
+    <t>OMS_CI_04</t>
+  </si>
+  <si>
+    <t>OMS_CI_05</t>
+  </si>
+  <si>
+    <t>OMS_CI_06</t>
+  </si>
+  <si>
+    <t>Online_Mobile_Store/PM/OnlineMobileStore_CHG.xlsx at DIV · samawagdy123/Online_Mobile_Store (github.com)</t>
+  </si>
+  <si>
+    <t>Online_Mobile_Store/PM/OnlineMobileStore_IMP.xlsx at DIV · samawagdy123/Online_Mobile_Store (github.com)</t>
+  </si>
+  <si>
+    <t>Online_Mobile_Store/PM/OnlineMobileStore_Review.xlsx at DIV · samawagdy123/Online_Mobile_Store (github.com)</t>
+  </si>
+  <si>
+    <t>https://github.com/samawagdy123/Online_Mobile_Store/blob/DIV/PM/OnlineMobileStore_PMP.docx</t>
+  </si>
+  <si>
+    <t>https://github.com/samawagdy123/Online_Mobile_Store/blob/DIV/Requirement/OnlineMobileStore_SRS.docx</t>
+  </si>
+  <si>
+    <t>https://github.com/samawagdy123/Online_Mobile_Store/blob/DIV/Requirement/OnlineMobileStore_SIQ.xlsx</t>
+  </si>
+  <si>
+    <t>Mohammed El-Kassas
+Mario Adel</t>
+  </si>
+  <si>
+    <t>/Online_Mobile_Store/Requirement/SRS</t>
+  </si>
+  <si>
+    <t>/Online_Mobile_Store/Requirement/SIQ</t>
+  </si>
+  <si>
+    <t>/Online_Mobile_Store/PM/OnlineMobileStore_CHG.xlsx</t>
+  </si>
+  <si>
+    <t>/Online_Mobile_Store/PM/OnlineMobileStore_Review.xlsx</t>
+  </si>
+  <si>
+    <t>/Online_Mobile_Store/PM/OnlineMobileStore_IMPxlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Request to Change </t>
+  </si>
+  <si>
+    <t>Approvid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Approvid </t>
+  </si>
+  <si>
+    <t>OMS_CI_07</t>
+  </si>
+  <si>
+    <t>v1.1</t>
+  </si>
+  <si>
+    <t>RTM</t>
+  </si>
+  <si>
+    <t>Salma Mohamed</t>
+  </si>
+  <si>
+    <t>Review</t>
   </si>
 </sst>
 </file>
@@ -104,7 +186,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +235,14 @@
       <family val="5"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Univers"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -177,10 +267,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -200,9 +291,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -227,11 +315,95 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Univers"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Univers"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Univers"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Univers"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -252,81 +424,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="1" tint="0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Univers"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Univers"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Univers"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Univers"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -389,6 +486,19 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="1" tint="0.34998626667073579"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -546,8 +656,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Inventory_List_Table" displayName="Inventory_List_Table" ref="A3:G28" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A3:G28" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Inventory_List_Table" displayName="Inventory_List_Table" ref="A3:G25" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A3:G25" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -557,13 +667,13 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ID" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Name" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{CD01D83F-9960-460F-8C66-E1B9FC62EA4C}" name="Owner" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Link" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Version" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Path" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Configuration level" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ID" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Name" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{CD01D83F-9960-460F-8C66-E1B9FC62EA4C}" name="Owner" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Link" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Version" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Path" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Configuration level" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark9 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -772,33 +882,34 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F3" zoomScale="84" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.125" style="5" customWidth="1"/>
-    <col min="2" max="3" width="22.5" style="9" customWidth="1"/>
-    <col min="4" max="4" width="47.875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="22.5" style="10" customWidth="1"/>
-    <col min="6" max="6" width="37.875" style="10" customWidth="1"/>
-    <col min="7" max="7" width="28.75" style="10" customWidth="1"/>
+    <col min="1" max="1" width="19.875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="22.5" style="8" customWidth="1"/>
+    <col min="3" max="3" width="43.625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="109.75" style="18" customWidth="1"/>
+    <col min="5" max="5" width="22.5" style="9" customWidth="1"/>
+    <col min="6" max="6" width="54.875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="28.75" style="5" customWidth="1"/>
     <col min="8" max="16384" width="8.625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="12" customFormat="1" ht="110.1" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:7" s="11" customFormat="1" ht="110.1" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="21"/>
     </row>
     <row r="2" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -806,290 +917,320 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="D2" s="17"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="G2" s="21"/>
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="11" t="s">
+      <c r="C3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="6"/>
+      <c r="C5" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="6"/>
+      <c r="C6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="6"/>
+      <c r="C7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="6"/>
+      <c r="C8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="6"/>
+      <c r="D9" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="6"/>
+      <c r="A10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="19"/>
+      <c r="E10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="7"/>
+      <c r="D11" s="20"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="6"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="7"/>
+      <c r="D12" s="20"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="6"/>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
-      <c r="D13" s="7"/>
+      <c r="D13" s="20"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="6"/>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
-      <c r="D14" s="7"/>
+      <c r="D14" s="20"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="6"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
-      <c r="D15" s="7"/>
+      <c r="D15" s="20"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="6"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
+      <c r="D16" s="20"/>
       <c r="E16" s="6"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="6"/>
-    </row>
-    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
+      <c r="D17" s="20"/>
       <c r="E17" s="6"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="6"/>
-    </row>
-    <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="7"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="6"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="7"/>
+      <c r="D19" s="20"/>
       <c r="E19" s="6"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="6"/>
-    </row>
-    <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
-      <c r="D20" s="7"/>
+      <c r="D20" s="20"/>
       <c r="E20" s="6"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="6"/>
-    </row>
-    <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
-      <c r="D21" s="7"/>
+      <c r="D21" s="20"/>
       <c r="E21" s="6"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="6"/>
-    </row>
-    <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
-      <c r="D22" s="7"/>
+      <c r="D22" s="20"/>
       <c r="E22" s="6"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="6"/>
-    </row>
-    <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
-      <c r="D23" s="7"/>
+      <c r="D23" s="20"/>
       <c r="E23" s="6"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="6"/>
-    </row>
-    <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
-      <c r="D24" s="7"/>
+      <c r="D24" s="20"/>
       <c r="E24" s="6"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="6"/>
-    </row>
-    <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
-      <c r="D25" s="7"/>
+      <c r="D25" s="20"/>
       <c r="E25" s="6"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="6"/>
-    </row>
-    <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="6"/>
-    </row>
-    <row r="27" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="6"/>
-    </row>
-    <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="6"/>
+      <c r="F25" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A4:G28">
-    <cfRule type="expression" dxfId="2" priority="16">
+  <conditionalFormatting sqref="A11:G25 A4:C10 E4:G10">
+    <cfRule type="expression" dxfId="10" priority="16">
       <formula>#REF!="Yes"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="17">
+    <cfRule type="expression" dxfId="9" priority="17">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1102,11 +1243,19 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the unit price of each item in this column" sqref="D3" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter company name in this cell" sqref="A2" xr:uid="{49791EBD-DD5B-4484-B3BA-6B061218151B}"/>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{A852C872-E8E8-4ECF-A9C9-E39F2C545FF6}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{0A310357-F56E-4854-8073-903A66A8284B}"/>
+    <hyperlink ref="D6" r:id="rId3" xr:uid="{4D90A08D-7C9D-420A-A73C-FD22BFDA8F47}"/>
+    <hyperlink ref="D7" r:id="rId4" display="https://github.com/samawagdy123/Online_Mobile_Store/blob/DIV/PM/OnlineMobileStore_CHG.xlsx" xr:uid="{94F74A59-D797-4346-A1B6-4001F5487705}"/>
+    <hyperlink ref="D8" r:id="rId5" display="https://github.com/samawagdy123/Online_Mobile_Store/blob/DIV/PM/OnlineMobileStore_IMP.xlsx" xr:uid="{2443A1F3-3360-4800-B5EA-071A7517BD46}"/>
+    <hyperlink ref="D9" r:id="rId6" display="https://github.com/samawagdy123/Online_Mobile_Store/blob/DIV/PM/OnlineMobileStore_Review.xlsx" xr:uid="{2620BF93-EAE0-4F17-8AFA-EB76BD27F479}"/>
+  </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="43" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="43" fitToHeight="0" orientation="portrait" r:id="rId7"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
ID:OMS-CIL-02-->update with docs in sprint 2&3
Add configuration items such as HLD, LLD, RTM, and CusReq.
</commit_message>
<xml_diff>
--- a/PM/OnlineMobileStore_CIL.xlsx
+++ b/PM/OnlineMobileStore_CIL.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007431E6-91D2-49C4-A4CB-93B3C427A39E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12344F9D-90E5-458F-912E-EAFE3532A341}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -154,9 +154,6 @@
     <t>/Online_Mobile_Store/PM/OnlineMobileStore_IMPxlsx</t>
   </si>
   <si>
-    <t xml:space="preserve">Request to Change </t>
-  </si>
-  <si>
     <t>Approvid</t>
   </si>
   <si>
@@ -166,9 +163,6 @@
     <t>OMS_CI_07</t>
   </si>
   <si>
-    <t>v1.1</t>
-  </si>
-  <si>
     <t>RTM</t>
   </si>
   <si>
@@ -176,6 +170,70 @@
   </si>
   <si>
     <t>Review</t>
+  </si>
+  <si>
+    <t>Online_Mobile_Store/PM/OnlineMobileStore_RTM.xlsx at main · samawagdy123/Online_Mobile_Store (github.com)</t>
+  </si>
+  <si>
+    <t>OMS_CI_08</t>
+  </si>
+  <si>
+    <t>OMS_CI_09</t>
+  </si>
+  <si>
+    <t>OMS_CI_10</t>
+  </si>
+  <si>
+    <t>Customer Requirments</t>
+  </si>
+  <si>
+    <t>Online_Mobile_Store/PM/OnlineMobileStore_CusReq.jpeg at main · samawagdy123/Online_Mobile_Store (github.com)</t>
+  </si>
+  <si>
+    <t>v2.1</t>
+  </si>
+  <si>
+    <t>v3.0</t>
+  </si>
+  <si>
+    <t>v2.0</t>
+  </si>
+  <si>
+    <t>Online_Mobile_Store/Design/OnlineMobileStore_Design_HLD.docx at main · samawagdy123/Online_Mobile_Store (github.com)</t>
+  </si>
+  <si>
+    <t>HLD</t>
+  </si>
+  <si>
+    <t>M.El-kassas
+Mario
+Salma Mohamed</t>
+  </si>
+  <si>
+    <t>/Online_Mobile_Store/PM/OnlineMobileStore_RTM.xlsx</t>
+  </si>
+  <si>
+    <t>/Online_Mobile_Store/PM/OnlineMobileStore_CusReq.xlsx</t>
+  </si>
+  <si>
+    <t>/Online_Mobile_Store/Design/OnlineMobileStore_DESIGN_HLD.xlsx</t>
+  </si>
+  <si>
+    <t>/Online_Mobile_Store/Design/OnlineMobileStore_DESIGN_LLD.xlsx</t>
+  </si>
+  <si>
+    <t>Sama Wagdy
+Salma Khaled
+Salma Mohammed</t>
+  </si>
+  <si>
+    <t>LLD</t>
+  </si>
+  <si>
+    <t>Online_Mobile_Store/Design/OnlineMobileStore_Design_LLD.docx at main · samawagdy123/Online_Mobile_Store (github.com)</t>
+  </si>
+  <si>
+    <t>Fixed</t>
   </si>
 </sst>
 </file>
@@ -271,7 +329,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -336,6 +394,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -884,8 +943,8 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F3" zoomScale="84" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="84" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -895,7 +954,7 @@
     <col min="3" max="3" width="43.625" style="8" customWidth="1"/>
     <col min="4" max="4" width="109.75" style="18" customWidth="1"/>
     <col min="5" max="5" width="22.5" style="9" customWidth="1"/>
-    <col min="6" max="6" width="54.875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="66.375" style="9" customWidth="1"/>
     <col min="7" max="7" width="28.75" style="5" customWidth="1"/>
     <col min="8" max="16384" width="8.625" style="3"/>
   </cols>
@@ -982,13 +1041,13 @@
         <v>31</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>34</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1011,7 +1070,7 @@
         <v>35</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1034,7 +1093,7 @@
         <v>36</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1057,7 +1116,7 @@
         <v>38</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1074,59 +1133,106 @@
         <v>29</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>37</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="5" t="s">
+    </row>
+    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="7"/>
+      <c r="B11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
@@ -1226,7 +1332,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A11:G25 A4:C10 E4:G10">
+  <conditionalFormatting sqref="A14:G25 A4:C13 E4:G13">
     <cfRule type="expression" dxfId="10" priority="16">
       <formula>#REF!="Yes"</formula>
     </cfRule>
@@ -1250,17 +1356,30 @@
     <hyperlink ref="D7" r:id="rId4" display="https://github.com/samawagdy123/Online_Mobile_Store/blob/DIV/PM/OnlineMobileStore_CHG.xlsx" xr:uid="{94F74A59-D797-4346-A1B6-4001F5487705}"/>
     <hyperlink ref="D8" r:id="rId5" display="https://github.com/samawagdy123/Online_Mobile_Store/blob/DIV/PM/OnlineMobileStore_IMP.xlsx" xr:uid="{2443A1F3-3360-4800-B5EA-071A7517BD46}"/>
     <hyperlink ref="D9" r:id="rId6" display="https://github.com/samawagdy123/Online_Mobile_Store/blob/DIV/PM/OnlineMobileStore_Review.xlsx" xr:uid="{2620BF93-EAE0-4F17-8AFA-EB76BD27F479}"/>
+    <hyperlink ref="D10" r:id="rId7" display="https://github.com/samawagdy123/Online_Mobile_Store/blob/main/PM/OnlineMobileStore_RTM.xlsx" xr:uid="{42C56440-A21D-40E9-A491-3A90E75B1AE5}"/>
+    <hyperlink ref="D11" r:id="rId8" display="https://github.com/samawagdy123/Online_Mobile_Store/blob/main/PM/OnlineMobileStore_CusReq.jpeg" xr:uid="{01D5F63F-0810-4A82-A4B6-6610FC487CB8}"/>
+    <hyperlink ref="D12" r:id="rId9" display="https://github.com/samawagdy123/Online_Mobile_Store/blob/main/Design/OnlineMobileStore_Design_HLD.docx" xr:uid="{B14E4646-3B54-4E4F-BCE2-E271C16BF8DC}"/>
+    <hyperlink ref="D13" r:id="rId10" display="https://github.com/samawagdy123/Online_Mobile_Store/blob/main/Design/OnlineMobileStore_Design_LLD.docx" xr:uid="{5E72A541-AEE3-410F-8063-B098D36AB828}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="43" fitToHeight="0" orientation="portrait" r:id="rId7"/>
+  <pageSetup scale="43" fitToHeight="0" orientation="portrait" r:id="rId11"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId12"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -1278,15 +1397,6 @@
     <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1602,6 +1712,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99D1F540-32A9-4ED6-9336-A9BD181B3061}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2651663D-B88E-4AD7-9DE9-C58C98743015}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1609,14 +1727,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
     <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99D1F540-32A9-4ED6-9336-A9BD181B3061}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>